<commit_message>
feat: update Excel files in ejemplos_api for improved data handling
</commit_message>
<xml_diff>
--- a/ejemplos_api/apocrifos.xlsx
+++ b/ejemplos_api/apocrifos.xlsx
@@ -9,7 +9,9 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <definedNames/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet1'!$A$1:$A$3</definedName>
+  </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
@@ -17,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,13 +30,22 @@
     <font>
       <b val="1"/>
     </font>
+    <font>
+      <color rgb="00FFFFFF"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00002060"/>
+        <bgColor rgb="00002060"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,9 +66,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -432,9 +446,12 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13" customWidth="1" min="1" max="1"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>cuit</t>
         </is>
@@ -455,6 +472,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:A3"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>